<commit_message>
modification du fichier contact_linkedin: EasyBank
</commit_message>
<xml_diff>
--- a/Contact_Linkedin.xlsx
+++ b/Contact_Linkedin.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t xml:space="preserve">Nom de la société</t>
   </si>
@@ -134,6 +134,15 @@
   </si>
   <si>
     <t xml:space="preserve">Dev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EasyBank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/posts/easybank-official_summerinternships-finance-marketing-activity-7200065600138682368-m-zZ?utm_source=share&amp;utm_medium=member_desktop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT</t>
   </si>
 </sst>
 </file>
@@ -337,10 +346,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -492,6 +501,17 @@
       </c>
       <c r="C13" s="0" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>